<commit_message>
update venn diagram notes
</commit_message>
<xml_diff>
--- a/venn-diam.xlsx
+++ b/venn-diam.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Dropbox/2017 Fall/amicus brief/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Documents/Amicus-Brief/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="3880" windowWidth="24960" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="5900" yWindow="460" windowWidth="24960" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>GENERAL COALITIONAL BEHAVIOR</t>
   </si>
@@ -67,6 +67,9 @@
   <si>
     <t>black, latino and asian file separately</t>
   </si>
+  <si>
+    <t>Note: the numbers in this venn diagram represent the briefs in the concurrance cases. There're total 75 separate briefs out of the 26 concurrance cases.</t>
+  </si>
 </sst>
 </file>
 
@@ -101,8 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,6 +1092,13 @@
     <dgm:pt modelId="{66A83EF3-61C8-3641-892A-4462E88E8151}" type="pres">
       <dgm:prSet presAssocID="{F45D6990-A728-274C-8757-BD3D42D16A8A}" presName="circ2" presStyleLbl="vennNode1" presStyleIdx="1" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FA64DBBF-D31C-5A4F-860C-CE8FEFF238C7}" type="pres">
       <dgm:prSet presAssocID="{F45D6990-A728-274C-8757-BD3D42D16A8A}" presName="circ2Tx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -1096,10 +1109,24 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5C63A745-C20D-9145-BEB0-322090B88B3E}" type="pres">
       <dgm:prSet presAssocID="{94C00AAA-AC00-814B-A32F-D987CE4B794D}" presName="circ3" presStyleLbl="vennNode1" presStyleIdx="2" presStyleCnt="3"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{EE63F017-3CF3-0B47-8403-5582DCBBB0C9}" type="pres">
       <dgm:prSet presAssocID="{94C00AAA-AC00-814B-A32F-D987CE4B794D}" presName="circ3Tx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -1110,6 +1137,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -3960,10 +3994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4058,7 +4092,30 @@
         <v>7</v>
       </c>
     </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C34:I35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>